<commit_message>
fix send of data
</commit_message>
<xml_diff>
--- a/base_datos/pedidos.xlsx
+++ b/base_datos/pedidos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,18 +521,613 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="n">
         <v>45000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:11:49</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:11:49</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alemana</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:17:15</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:21:10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:23:41</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Ranchera</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G12" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:23:41</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alemana</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G13" t="n">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:24:23</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G15" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:25:29</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:30:07</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:33:24</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G21" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:39:57</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F23" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G23" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:41:01</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Ranchera</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G25" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:42:00</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:42:58</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G29" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:45:14</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G31" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change line 93 in file mesero.py
</commit_message>
<xml_diff>
--- a/base_datos/pedidos.xlsx
+++ b/base_datos/pedidos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,18 +1198,59 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
-      <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
       <c r="G36" t="n">
         <v>1600</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-03-01 01:57:52</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G37" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr"/>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="n">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en diseño y respuesta
</commit_message>
<xml_diff>
--- a/base_datos/pedidos.xlsx
+++ b/base_datos/pedidos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,18 +1239,450 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
-      <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
       <c r="G38" t="n">
         <v>20000</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:02:15</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:08:43</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G41" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:09:45</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>camilo</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G43" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:19:10</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Combinado</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Perro Caliente</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G45" t="n">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:19:10</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Gemelo</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Perro Caliente</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" t="n">
+        <v>9000</v>
+      </c>
+      <c r="G46" t="n">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:19:10</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Suizo</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Perro Caliente</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>3</v>
+      </c>
+      <c r="F47" t="n">
+        <v>12000</v>
+      </c>
+      <c r="G47" t="n">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G48" t="n">
+        <v>63000</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:25:40</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Sencilla</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>3</v>
+      </c>
+      <c r="F49" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G49" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:25:40</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Mixta</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>3</v>
+      </c>
+      <c r="F50" t="n">
+        <v>17000</v>
+      </c>
+      <c r="G50" t="n">
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:25:40</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Combinada</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" t="n">
+        <v>12000</v>
+      </c>
+      <c r="G51" t="n">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="G52" t="n">
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:29:28</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Ranchera</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>3</v>
+      </c>
+      <c r="F53" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G53" t="n">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:29:28</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Combinada</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>12000</v>
+      </c>
+      <c r="G54" t="n">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-03-01 02:29:28</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>benichi</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Salchipollo</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Salchipapas</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="n">
+        <v>15000</v>
+      </c>
+      <c r="G55" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr"/>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="inlineStr"/>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="n">
+        <v>99000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>